<commit_message>
remove some value for excel
</commit_message>
<xml_diff>
--- a/app/Downloads/Accounts.xlsx
+++ b/app/Downloads/Accounts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>id</t>
   </si>
@@ -29,12 +29,6 @@
     <t>email_verified_at</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>remember_token</t>
-  </si>
-  <si>
     <t>created_at</t>
   </si>
   <si>
@@ -47,49 +41,46 @@
     <t>badlonmazeclarion@gmail.com</t>
   </si>
   <si>
-    <t>2023-06-08T18:20:30.000000Z</t>
-  </si>
-  <si>
-    <t>Maze Clarion</t>
-  </si>
-  <si>
-    <t>badlonmazeclarion1@gmail.com</t>
-  </si>
-  <si>
-    <t>2023-06-08T23:50:09.000000Z</t>
-  </si>
-  <si>
-    <t>Maze711</t>
-  </si>
-  <si>
-    <t>Mazee711@gmail.com</t>
-  </si>
-  <si>
-    <t>2023-06-08T23:53:45.000000Z</t>
-  </si>
-  <si>
-    <t>2023-06-09T21:04:17.000000Z</t>
-  </si>
-  <si>
-    <t>Maze</t>
-  </si>
-  <si>
-    <t>Mazee@gmail.com</t>
-  </si>
-  <si>
-    <t>2023-06-09T17:21:39.000000Z</t>
-  </si>
-  <si>
-    <t>2023-06-09T21:04:05.000000Z</t>
-  </si>
-  <si>
-    <t>Mykall</t>
-  </si>
-  <si>
-    <t>mike@gmail.com</t>
-  </si>
-  <si>
-    <t>2023-06-09T22:54:12.000000Z</t>
+    <t>2023-06-09T09:20:30.000000Z</t>
+  </si>
+  <si>
+    <t>badlonmaze@gmail.com</t>
+  </si>
+  <si>
+    <t>2023-06-09T11:08:16.000000Z</t>
+  </si>
+  <si>
+    <t>badlon@gmail.com</t>
+  </si>
+  <si>
+    <t>2023-06-09T11:09:40.000000Z</t>
+  </si>
+  <si>
+    <t>Mazeu</t>
+  </si>
+  <si>
+    <t>maze@gmail.com</t>
+  </si>
+  <si>
+    <t>2023-06-09T11:25:51.000000Z</t>
+  </si>
+  <si>
+    <t>Kirk J-Son Matic</t>
+  </si>
+  <si>
+    <t>kirk@gmail.com</t>
+  </si>
+  <si>
+    <t>2023-06-09T10:35:08.000000Z</t>
+  </si>
+  <si>
+    <t>Rodel Cuyag</t>
+  </si>
+  <si>
+    <t>rodel@gmail.com</t>
+  </si>
+  <si>
+    <t>2023-06-11T01:05:32.000000Z</t>
   </si>
 </sst>
 </file>
@@ -429,7 +420,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,7 +428,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,96 +447,107 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="F5" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>24</v>
+      <c r="F7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>